<commit_message>
Select tables: Add switch to use rows for initial age (i.e. a row describes one person)
</commit_message>
<xml_diff>
--- a/data-raw/US/Basic_Select-Ultimate/USA_1965-70_Basic_Select_Ultimate.xlsx
+++ b/data-raw/US/Basic_Select-Ultimate/USA_1965-70_Basic_Select_Ultimate.xlsx
@@ -44,26 +44,8 @@
     <t xml:space="preserve">USA 1965-70 (Modified) Basic Select-Ultimate Tables</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Male Age last Birthday, per 1000, i.e. 1000 q_x 
-Source: Transactions SoA 1977 Vol.29, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://www.soa.org/Library/Research/Transactions-Of-Society-Of-Actuaries/1977/January/tsa77v295.pdf</t>
-    </r>
+    <t xml:space="preserve">Male Age last Birthday, per 1000, i.e. 1000 q_x 
+Source: Transactions SoA 1977 Vol.29, http://www.soa.org/Library/Research/Transactions-Of-Society-Of-Actuaries/1977/January/tsa77v295.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Female Age last Birthday, per 1000, i.e. 1000 q_x 
@@ -294,7 +276,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,7 +371,7 @@
       <selection pane="topLeft" activeCell="R5" activeCellId="0" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="9.47"/>
@@ -5336,7 +5318,7 @@
       <selection pane="topLeft" activeCell="R90" activeCellId="0" sqref="R90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="9.47"/>
@@ -10279,7 +10261,7 @@
       <selection pane="topLeft" activeCell="R90" activeCellId="0" sqref="R90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="9.47"/>
@@ -15170,7 +15152,7 @@
     <mergeCell ref="A2:Q2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://www.soa.org/Library/Research/Transactions-Of-Society-Of-Actuaries/1977/January/tsa77v295.pdf"/>
+    <hyperlink ref="A2" r:id="rId1" display="Male Age last Birthday, per 1000, i.e. 1000 q_x &#10;Source: Transactions SoA 1977 Vol.29, http://www.soa.org/Library/Research/Transactions-Of-Society-Of-Actuaries/1977/January/tsa77v295.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -15189,11 +15171,11 @@
   </sheetPr>
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R90" activeCellId="0" sqref="R90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="9.47"/>

</xml_diff>